<commit_message>
switch to static level shifting
</commit_message>
<xml_diff>
--- a/pin-assignments.xlsx
+++ b/pin-assignments.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Nextcloud\Documents\Projects\nixieclock\nixie-clock-ice\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Nextcloud\Documents\Projects\nixieclock\nixie-clock-ice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386EDB0A-660E-498F-BD76-9D2702B47A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1688AF15-6843-4DD3-B4A8-CDA61C484723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{61DDA8EF-D3AB-45D9-ADB5-848A3329CB87}"/>
+    <workbookView xWindow="15360" yWindow="4284" windowWidth="25644" windowHeight="15588" xr2:uid="{61DDA8EF-D3AB-45D9-ADB5-848A3329CB87}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1134,27 +1134,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{048455D2-8E6B-4BC7-A693-16ADCA598B53}">
   <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
       <selection activeCell="A41" sqref="A41"/>
-      <selection pane="topRight"/>
+      <selection pane="topRight" activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.62890625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.15625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7890625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.9453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7890625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.1015625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="115.26171875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="115.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1346,7 +1346,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1506,7 +1506,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1538,7 +1538,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1570,7 +1570,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1634,7 +1634,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1666,7 +1666,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1698,7 +1698,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -1762,7 +1762,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -1794,7 +1794,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -1858,7 +1858,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -1890,7 +1890,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -1922,7 +1922,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -1986,7 +1986,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -2018,7 +2018,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -2050,7 +2050,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:10" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -2114,7 +2114,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -2178,7 +2178,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -2274,7 +2274,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -2338,7 +2338,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -2370,7 +2370,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -2402,7 +2402,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -2434,7 +2434,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -2466,7 +2466,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -2498,7 +2498,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -2594,7 +2594,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -2626,7 +2626,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -2658,7 +2658,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -2684,13 +2684,13 @@
         <v>57</v>
       </c>
       <c r="I48" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="J48" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -2716,13 +2716,13 @@
         <v>57</v>
       </c>
       <c r="I49" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="J49" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -2786,7 +2786,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -2818,7 +2818,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -2850,7 +2850,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -2882,7 +2882,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -2914,7 +2914,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -2946,7 +2946,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -2978,7 +2978,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -3010,7 +3010,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -3042,7 +3042,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -3074,7 +3074,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -3106,7 +3106,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -3138,7 +3138,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -3170,7 +3170,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -3199,7 +3199,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -3228,7 +3228,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -3257,7 +3257,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -3286,7 +3286,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -3315,7 +3315,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -3344,7 +3344,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -3373,7 +3373,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -3402,7 +3402,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -3434,7 +3434,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -3466,7 +3466,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -3498,7 +3498,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -3530,7 +3530,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -3562,7 +3562,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -3594,7 +3594,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -3626,7 +3626,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -3658,7 +3658,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -3690,7 +3690,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" s="3">
         <v>80</v>
       </c>

</xml_diff>

<commit_message>
update ADC pinout for improved routing
</commit_message>
<xml_diff>
--- a/pin-assignments.xlsx
+++ b/pin-assignments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Nextcloud\Documents\Projects\nixieclock\nixie-clock-ice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB4C951-C8C5-4D60-89F6-97AD8A88BA4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00BF6CDD-FE27-41B9-9DFF-88BC5D328A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{61DDA8EF-D3AB-45D9-ADB5-848A3329CB87}"/>
+    <workbookView xWindow="8448" yWindow="6468" windowWidth="25656" windowHeight="15588" xr2:uid="{61DDA8EF-D3AB-45D9-ADB5-848A3329CB87}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -696,7 +696,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -715,8 +715,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor theme="6" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor theme="6" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -733,11 +745,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </left>
+      <right style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -748,11 +775,69 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="13">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -820,14 +905,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B8DDC3D1-B6B2-4773-BAE3-53756E759D9B}" name="Table1" displayName="Table1" ref="A1:J81" totalsRowShown="0">
   <autoFilter ref="A1:J81" xr:uid="{B8DDC3D1-B6B2-4773-BAE3-53756E759D9B}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{973649EE-E7D7-444A-B6E8-0C168ED11786}" name="pico iCE pin" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{973649EE-E7D7-444A-B6E8-0C168ED11786}" name="pico iCE pin" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{F5653507-11B6-4725-89A0-0D52D7FE48D4}" name="iCE 40 pin"/>
     <tableColumn id="3" xr3:uid="{62EAA3B7-CDFA-4331-AA91-B5A19A4C9C69}" name="iCE 40 config"/>
     <tableColumn id="4" xr3:uid="{EE7FDF9B-97D2-4ADF-9BB7-2B25579CE898}" name="iCE 40 bank"/>
-    <tableColumn id="5" xr3:uid="{65394EF3-41D0-4EA1-B6F6-F3D44BD72055}" name="iCE 40 ID" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{65394EF3-41D0-4EA1-B6F6-F3D44BD72055}" name="iCE 40 ID" dataDxfId="11"/>
     <tableColumn id="6" xr3:uid="{CEFAB0DD-E9AA-433F-8309-BC2DA89CD8A4}" name="RP2040 pin"/>
     <tableColumn id="11" xr3:uid="{0788CCF3-2736-4162-BDED-CC62F0E680D7}" name="RP2040 ID"/>
-    <tableColumn id="8" xr3:uid="{2D3BF530-0CE5-4C3C-A254-B6F38E7E69AF}" name="RP2040 config" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{2D3BF530-0CE5-4C3C-A254-B6F38E7E69AF}" name="RP2040 config" dataDxfId="10"/>
     <tableColumn id="9" xr3:uid="{8B749DA2-6FA0-44A0-9521-2C507833EE62}" name="net"/>
     <tableColumn id="10" xr3:uid="{AB262432-1C8B-4560-A17E-3D18C1343AA3}" name="description"/>
   </tableColumns>
@@ -1450,7 +1535,7 @@
         <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1467,11 +1552,11 @@
       <c r="H10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I10" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10" t="s">
-        <v>201</v>
+      <c r="I10" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -1499,11 +1584,11 @@
       <c r="H11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I11" t="s">
-        <v>15</v>
-      </c>
-      <c r="J11" t="s">
-        <v>202</v>
+      <c r="I11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -1514,7 +1599,7 @@
         <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1531,11 +1616,11 @@
       <c r="H12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I12" t="s">
-        <v>16</v>
-      </c>
-      <c r="J12" t="s">
-        <v>203</v>
+      <c r="I12" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -1563,10 +1648,10 @@
       <c r="H13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="9" t="s">
         <v>204</v>
       </c>
     </row>
@@ -1578,7 +1663,7 @@
         <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1595,11 +1680,11 @@
       <c r="H14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I14" t="s">
-        <v>18</v>
-      </c>
-      <c r="J14" t="s">
-        <v>205</v>
+      <c r="I14" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -1610,7 +1695,7 @@
         <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1627,11 +1712,11 @@
       <c r="H15" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I15" t="s">
-        <v>42</v>
-      </c>
-      <c r="J15" t="s">
-        <v>206</v>
+      <c r="I15" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -1659,11 +1744,11 @@
       <c r="H16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J16" t="s">
-        <v>207</v>
+      <c r="I16" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -1691,11 +1776,11 @@
       <c r="H17" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I17" t="s">
-        <v>19</v>
-      </c>
-      <c r="J17" t="s">
-        <v>208</v>
+      <c r="I17" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -1770,7 +1855,7 @@
         <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1787,11 +1872,11 @@
       <c r="H20" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I20" t="s">
-        <v>129</v>
-      </c>
-      <c r="J20" t="s">
-        <v>209</v>
+      <c r="I20" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -1802,7 +1887,7 @@
         <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1819,11 +1904,11 @@
       <c r="H21" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I21" t="s">
-        <v>123</v>
-      </c>
-      <c r="J21" t="s">
-        <v>210</v>
+      <c r="I21" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="J21" s="9" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -1883,11 +1968,11 @@
       <c r="H23" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I23" t="s">
-        <v>125</v>
-      </c>
-      <c r="J23" t="s">
-        <v>211</v>
+      <c r="I23" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -2107,11 +2192,11 @@
       <c r="H30" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I30" t="s">
-        <v>33</v>
-      </c>
-      <c r="J30" t="s">
-        <v>212</v>
+      <c r="I30" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="J30" s="9" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
@@ -2139,11 +2224,11 @@
       <c r="H31" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I31" t="s">
-        <v>34</v>
-      </c>
-      <c r="J31" t="s">
-        <v>213</v>
+      <c r="I31" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J31" s="8" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
@@ -2154,7 +2239,7 @@
         <v>48</v>
       </c>
       <c r="C32" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="D32">
         <v>2</v>
@@ -2172,10 +2257,10 @@
         <v>26</v>
       </c>
       <c r="I32" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J32" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
@@ -3723,12 +3808,44 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:I81">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="GND">
+  <conditionalFormatting sqref="B2:I9 B10:H17 B18:I19 B20:H21 B22:I22 B23:H23 B24:I29 B30:H31 B32:I81">
+    <cfRule type="containsText" dxfId="9" priority="31" operator="containsText" text="GND">
       <formula>NOT(ISERROR(SEARCH("GND",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="8" priority="32" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",B2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I10:I17">
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="GND">
+      <formula>NOT(ISERROR(SEARCH("GND",I10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",I10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I20:I21">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="GND">
+      <formula>NOT(ISERROR(SEARCH("GND",I20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",I20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I23">
+    <cfRule type="containsText" dxfId="3" priority="21" operator="containsText" text="GND">
+      <formula>NOT(ISERROR(SEARCH("GND",I23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="22" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",I23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I30:I31">
+    <cfRule type="containsText" dxfId="1" priority="9" operator="containsText" text="GND">
+      <formula>NOT(ISERROR(SEARCH("GND",I30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="10" operator="containsText" text="N/A">
+      <formula>NOT(ISERROR(SEARCH("N/A",I30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>